<commit_message>
Agregado de nueva información de plantas medicinales. Update: Archivo de requirements.txt.
</commit_message>
<xml_diff>
--- a/Backend/src/PlantasMedicinalesDataset.xlsx
+++ b/Backend/src/PlantasMedicinalesDataset.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="332">
   <si>
     <t>Nombre Común</t>
   </si>
@@ -44,6 +44,39 @@
   </si>
   <si>
     <t>Otros antecedentes</t>
+  </si>
+  <si>
+    <t>Tipo de planta</t>
+  </si>
+  <si>
+    <t>Altura</t>
+  </si>
+  <si>
+    <t>Hojas</t>
+  </si>
+  <si>
+    <t>flores</t>
+  </si>
+  <si>
+    <t>Periodo de vida</t>
+  </si>
+  <si>
+    <t>Temperatura ideal</t>
+  </si>
+  <si>
+    <t>Exposición solar</t>
+  </si>
+  <si>
+    <t>Suelo</t>
+  </si>
+  <si>
+    <t>Propagación</t>
+  </si>
+  <si>
+    <t>Riego</t>
+  </si>
+  <si>
+    <t>Cosecha</t>
   </si>
   <si>
     <t>Tomillo</t>
@@ -54,12 +87,17 @@
   <si>
     <t>malestares digestivos (digestiones difíciles de tipo crónico
 (dispepsia), diarrea, cólicos, flatulencia, vómitos); parásitos intestinales;
-malestares respiratorios (tos, catarro, bronquitis, amigdalitis, resfríos). / heridas, eccemas, gingivitis, mal aliento; dolores reumáticos.
-Usar la misma infusión en lavados, compresas o gargarismos.</t>
+malestares respiratorios (tos, catarro, bronquitis, amigdalitis, resfríos). / heridas, eccemas, gingivitis, mal aliento; dolores reumáticos.</t>
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
-hervida: beber 1 taza 3 veces al día. / Usar la misma infusión en lavados, compresas o gargarismos.</t>
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>antiespasmodico / antiséptico / antitusivo / astringente / antibacteriano / 
@@ -81,6 +119,40 @@
 tópica tiene alguna evidencia científica.</t>
   </si>
   <si>
+    <t>Subarbusto</t>
+  </si>
+  <si>
+    <t>40 cm</t>
+  </si>
+  <si>
+    <t>verde-grisáceas</t>
+  </si>
+  <si>
+    <t>Púrpura, rosada o blanca</t>
+  </si>
+  <si>
+    <t>Perenne</t>
+  </si>
+  <si>
+    <t>8ºC-24°C
+Resiste heladas y sequias</t>
+  </si>
+  <si>
+    <t>Soleado</t>
+  </si>
+  <si>
+    <t>Pedregosos, bien drenados</t>
+  </si>
+  <si>
+    <t>Semillas, esquejes</t>
+  </si>
+  <si>
+    <t>1 vez por semana</t>
+  </si>
+  <si>
+    <t>Primavera, Verano-Otoño</t>
+  </si>
+  <si>
     <t>Melissa</t>
   </si>
   <si>
@@ -108,7 +180,11 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
-hervida: beber 1 taza 3 veces al día. / La misma infusión se usa en lavados o compresas.</t>
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t xml:space="preserve">antiespasmódico / antiviral / carminativo / estomacal / sedante </t>
@@ -130,6 +206,31 @@
 sedante en trastornos del sueño tiene alguna evidencia científica.</t>
   </si>
   <si>
+    <t>Hierba</t>
+  </si>
+  <si>
+    <t>90 cm</t>
+  </si>
+  <si>
+    <t>Verde oscuro</t>
+  </si>
+  <si>
+    <t>Blancas, rosadas o amarillas</t>
+  </si>
+  <si>
+    <t>18°C-25°C
+Sensible a heladas</t>
+  </si>
+  <si>
+    <t>Soleado o semisombra</t>
+  </si>
+  <si>
+    <t>Fértiles, bien drenados</t>
+  </si>
+  <si>
+    <t>Antes de floración</t>
+  </si>
+  <si>
     <t>Toronjil Cuyano</t>
   </si>
   <si>
@@ -158,7 +259,13 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
-recién hervida: beber 1 taza 3 veces al día. / La misma infusión sirve para uso externo en lavados.</t>
+recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
+recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
+recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
+recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
+recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
+recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de sumidades floridas para 1 litro de agua
+recién hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>diaforético / expectorante / febrífugo / balsámico / emenagogo / antidiarreico / digestivo</t>
@@ -181,6 +288,28 @@
 apetito tiene alguna evidencia científica.</t>
   </si>
   <si>
+    <t>80 cm</t>
+  </si>
+  <si>
+    <t>Verde-grisáceas</t>
+  </si>
+  <si>
+    <t>Blancas o crema</t>
+  </si>
+  <si>
+    <t>15°C-20°C
+Sensible a heladas, resiste sequías</t>
+  </si>
+  <si>
+    <t>Ricos materia orgánica, bien drenados</t>
+  </si>
+  <si>
+    <t>2 veces por semana</t>
+  </si>
+  <si>
+    <t>Durante floración</t>
+  </si>
+  <si>
     <t>Poleo</t>
   </si>
   <si>
@@ -208,6 +337,9 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
 hervida: beber 1 taza 3 veces en el día.</t>
   </si>
   <si>
@@ -232,6 +364,34 @@
     <t>su uso está avalado sólo por la tradición.</t>
   </si>
   <si>
+    <t>45 cm</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>Blanco a violáceo</t>
+  </si>
+  <si>
+    <t>10°C-35°C
+Resiste heladas</t>
+  </si>
+  <si>
+    <t>Soleado-semisombra</t>
+  </si>
+  <si>
+    <t>Calcáreos, ligeros y fértiles</t>
+  </si>
+  <si>
+    <t>Semillas, estolones</t>
+  </si>
+  <si>
+    <t>3 veces por semana</t>
+  </si>
+  <si>
+    <t>Todo el año</t>
+  </si>
+  <si>
     <t>Albahaca</t>
   </si>
   <si>
@@ -244,10 +404,17 @@
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
 hervida: beber 1 taza 3 veces en el día.
-Como laxante, usar en ayunas y antes del almuerzo; / La misma infusión sirve para lavar heridas; el jugo fresco de hojas para el acné;
-para reumatismo hacer friegas: dejar macerar hojas frescas en alcohol o
-aguardiente por 10-15 días, poner al sol un rato cada día, luego filtrar y usar en
-frotaciones locales 2 ó 3 veces en el día.</t>
+Como laxante, usar en ayunas y antes del almuerzo / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día.
+Como laxante, usar en ayunas y antes del almuerzo / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día.
+Como laxante, usar en ayunas y antes del almuerzo / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día.
+Como laxante, usar en ayunas y antes del almuerzo / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día.
+Como laxante, usar en ayunas y antes del almuerzo / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces en el día.
+Como laxante, usar en ayunas y antes del almuerzo;</t>
   </si>
   <si>
     <t>digestivo / carminativo / antiespasmódico / antimicrobiano / emenagogo / laxante</t>
@@ -267,6 +434,28 @@
 científica.</t>
   </si>
   <si>
+    <t>50 cm</t>
+  </si>
+  <si>
+    <t>Verde-violáceo</t>
+  </si>
+  <si>
+    <t>Blancas, rosadas a púrpura</t>
+  </si>
+  <si>
+    <t>Anual</t>
+  </si>
+  <si>
+    <t>20°C-25°C
+Sensible a heladas</t>
+  </si>
+  <si>
+    <t>Ricos en materia orgánica, arenosos o francos</t>
+  </si>
+  <si>
+    <t>Antes-durante floración</t>
+  </si>
+  <si>
     <t>Diente de León</t>
   </si>
   <si>
@@ -279,6 +468,10 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para las raíces hacer una decocción,
+hirviendo 1 cucharada por 10 minutos. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para las raíces hacer una decocción,
+hirviendo 1 cucharada por 10 minutos. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
 hervida: beber 1 taza 3 veces al día. Para las raíces hacer una decocción,
 hirviendo 1 cucharada por 10 minutos.</t>
   </si>
@@ -299,6 +492,22 @@
     <t>sus efectos tienen alguna evidencia científica.</t>
   </si>
   <si>
+    <t>Amarillas</t>
+  </si>
+  <si>
+    <t>0°C-35°C
+Resiste heladas</t>
+  </si>
+  <si>
+    <t>Ricos en materia orgánica bien drenados</t>
+  </si>
+  <si>
+    <t>Semillas y división de matas</t>
+  </si>
+  <si>
+    <t>Primavera-Otoño</t>
+  </si>
+  <si>
     <t>Menta Piperita</t>
   </si>
   <si>
@@ -324,6 +533,7 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada de vegetal (ó 6 a 8 hojas frescas) para 1
+litro de agua recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de vegetal (ó 6 a 8 hojas frescas) para 1
 litro de agua recién hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
@@ -342,6 +552,25 @@
 utensilios de aluminio.</t>
   </si>
   <si>
+    <t>Púrpura</t>
+  </si>
+  <si>
+    <t>0°C-32°C
+Resiste heladas</t>
+  </si>
+  <si>
+    <t>Soleado a semisombra</t>
+  </si>
+  <si>
+    <t>Húmedos y bien drenados</t>
+  </si>
+  <si>
+    <t>Rizomas, brotes laterales, esquejes, y semillas</t>
+  </si>
+  <si>
+    <t>Inicio floración</t>
+  </si>
+  <si>
     <t>Salvia</t>
   </si>
   <si>
@@ -370,7 +599,13 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
-hervida: beber 1 taza 3 veces al día. / Usar la misma infusión en lavados y gargarismos.</t>
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>antiespasmódico / antibacteriano / antisudoral / diurético / emenagogo / sedante / tocolítico</t>
@@ -393,6 +628,29 @@
 tienen alguna evidencia científica.</t>
   </si>
   <si>
+    <t>Sub-arbusto</t>
+  </si>
+  <si>
+    <t>70 cm</t>
+  </si>
+  <si>
+    <t>Blanco a violáceas</t>
+  </si>
+  <si>
+    <t>10°C-35°C
+Resiste sequías</t>
+  </si>
+  <si>
+    <t>Calcáreos, fértiles y bien drenados</t>
+  </si>
+  <si>
+    <t>Semillas, esquejes, estolones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Antes y durante floración</t>
+  </si>
+  <si>
     <t>Ajenjo</t>
   </si>
   <si>
@@ -432,6 +690,22 @@
 utensilios de aluminio.</t>
   </si>
   <si>
+    <t>130 cm</t>
+  </si>
+  <si>
+    <t>Amarillo</t>
+  </si>
+  <si>
+    <t>5°C-35°C
+Resiste heladas y sequías</t>
+  </si>
+  <si>
+    <t>Fértiles y bien drenados</t>
+  </si>
+  <si>
+    <t>Durante la floración</t>
+  </si>
+  <si>
     <t>Lavanda</t>
   </si>
   <si>
@@ -458,11 +732,27 @@
 y bronquitis. / dolores reumáticos.</t>
   </si>
   <si>
-    <t>La infusión se prepara con 1 cucharada de vegetal para 1 litro de agua recién
+    <t xml:space="preserve">La infusión se prepara con 1 cucharada de vegetal para 1 litro de agua recién
 hervida: beber 1 taza 3 veces al día. Para vahos (inhalaciones) preparar una
 decocción o cocimiento con 1 cucharada del vegetal para 1 litro de agua, calentar
-hasta ebullición y luego inhalar varias veces mientras el vapor se desprende. / Para baños se prepara con 2 a 5 cucharadas de flores para 20 litros de agua
-caliente.</t>
+hasta ebullición y luego inhalar varias veces mientras el vapor se desprende.  Para baños se prepara con 2 a 5 cucharadas de flores para 20 litros de agua
+caliente. / La infusión se prepara con 1 cucharada de vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para vahos (inhalaciones) preparar una
+decocción o cocimiento con 1 cucharada del vegetal para 1 litro de agua, calentar
+hasta ebullición y luego inhalar varias veces mientras el vapor se desprende.  Para baños se prepara con 2 a 5 cucharadas de flores para 20 litros de agua
+caliente. / La infusión se prepara con 1 cucharada de vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para vahos (inhalaciones) preparar una
+decocción o cocimiento con 1 cucharada del vegetal para 1 litro de agua, calentar
+hasta ebullición y luego inhalar varias veces mientras el vapor se desprende.  Para baños se prepara con 2 a 5 cucharadas de flores para 20 litros de agua
+caliente. / La infusión se prepara con 1 cucharada de vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para vahos (inhalaciones) preparar una
+decocción o cocimiento con 1 cucharada del vegetal para 1 litro de agua, calentar
+hasta ebullición y luego inhalar varias veces mientras el vapor se desprende. Para baños se prepara con 2 a 5 cucharadas de flores para 20 litros de agua
+caliente.  Para baños se prepara con 2 a 5 cucharadas de flores para 20 litros de agua
+caliente. / La infusión se prepara con 1 cucharada de vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para vahos (inhalaciones) preparar una
+decocción o cocimiento con 1 cucharada del vegetal para 1 litro de agua, calentar
+hasta ebullición y luego inhalar varias veces mientras el vapor se desprende. </t>
   </si>
   <si>
     <t>antiespasmódico / carminativo / sedante / balsamico / anti-inflamatorio</t>
@@ -479,6 +769,25 @@
 utensilios de aluminio.</t>
   </si>
   <si>
+    <t>Arbusto</t>
+  </si>
+  <si>
+    <t>1 m</t>
+  </si>
+  <si>
+    <t>Azul-violáceos</t>
+  </si>
+  <si>
+    <t>20°C a 30°C
+Resiste heladas</t>
+  </si>
+  <si>
+    <t>Ligeros, arenosos y bien drenados</t>
+  </si>
+  <si>
+    <t>Semillas y esquejes</t>
+  </si>
+  <si>
     <t>Romero</t>
   </si>
   <si>
@@ -508,6 +817,13 @@
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
 hervida: beber 1 taza 3 veces al día. / Para aplicación local se usa la misma infusión en lavado y compresas. Para baños
+usar 3 a 4 cucharadas en 20 litros de agua caliente. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. Para aplicación local se usa la misma infusión en lavado y compresas. Para baños
 usar 3 a 4 cucharadas en 20 litros de agua caliente.</t>
   </si>
   <si>
@@ -529,6 +845,19 @@
 inflamatorio tienen alguna evidencia científica.</t>
   </si>
   <si>
+    <t>2 m</t>
+  </si>
+  <si>
+    <t>Azuladas, rosadas o blancas</t>
+  </si>
+  <si>
+    <t>20°C-30°C
+Sensible a heladas-resiste sequías</t>
+  </si>
+  <si>
+    <t>Calcáreos, bien drenados</t>
+  </si>
+  <si>
     <t>Ruda</t>
   </si>
   <si>
@@ -555,6 +884,9 @@
   </si>
   <si>
     <t>La infusión se prepara con una 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con una 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con una 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con una 1 cucharada del vegetal para 1 litro de agua recién
 hervida: beber 1 taza 3 veces al día. / La infusión se prepara con una 1 cucharada del vegetal para 1 litro de agua recién
 hervida: beber 1 taza 3 veces al día.</t>
   </si>
@@ -578,6 +910,23 @@
 utensilios de aluminio.</t>
   </si>
   <si>
+    <t>Verde azulado</t>
+  </si>
+  <si>
+    <t>Amarillo y verde en el centro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15°C-25°C
+Resiste heladas-sequía
+</t>
+  </si>
+  <si>
+    <t>Fértiles, ligeros</t>
+  </si>
+  <si>
+    <t>Antes de la floración</t>
+  </si>
+  <si>
     <t>Matico</t>
   </si>
   <si>
@@ -609,8 +958,11 @@
   <si>
     <t xml:space="preserve">
 La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
-hervida: beber 1 taza 3 veces al día. / La misma infusión sirve para lavar heridas y en compresas para contusiones y
-hematomas (moretones).</t>
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. La misma infusión sirve para lavar heridas y en compresas para contusiones y
+hematomas (moretones). / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. </t>
   </si>
   <si>
     <t>analgésico / antimicótico / cicatrizante / anti-inflamatorio</t>
@@ -628,6 +980,16 @@
     <t>su efecto cicatrizante tiene alguna evidencia científica.</t>
   </si>
   <si>
+    <t>4 m</t>
+  </si>
+  <si>
+    <t>Amarillo-anaranjado</t>
+  </si>
+  <si>
+    <t>20°C-38°C
+Resiste heladas</t>
+  </si>
+  <si>
     <t>Caléndula</t>
   </si>
   <si>
@@ -653,9 +1015,14 @@
 pañal, eczemas); hemorroides; infecciones vaginales por hongos. </t>
   </si>
   <si>
-    <t xml:space="preserve">La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
-agua recién hervida: beber 1 taza 3 veces al día. / Usar la misma infusión en lavados y compresas; también se puede usar la tintura y
-la pomada. </t>
+    <t>La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
+agua recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
+agua recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
+agua recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
+agua recién hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
+agua recién hervida: beber 1 taza 3 veces al día. Usar la misma infusión en lavados y compresas; también se puede usar la tintura y
+la pomada. / La infusión se prepara con 1 cucharada de flores frescas o secas para 1 litro de
+agua recién hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>antiespasmódico / antibacteriano / emenagogo / digestivo / cicatrizante / anti-inflamatorio</t>
@@ -676,6 +1043,22 @@
 uso externo tiene alguna evidencia científica.</t>
   </si>
   <si>
+    <t>60 cm</t>
+  </si>
+  <si>
+    <t>Amarillas a naranjo</t>
+  </si>
+  <si>
+    <t>18°C-24°C
+Resiste heladas y sequías</t>
+  </si>
+  <si>
+    <t>Bien drenados</t>
+  </si>
+  <si>
+    <t>Semillas</t>
+  </si>
+  <si>
     <t>Manzanilla</t>
   </si>
   <si>
@@ -704,14 +1087,19 @@
   </si>
   <si>
     <t>La infusión se prepara con una cucharada de flores para 1 litro agua recién
-hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. / Usar la misma infusión como gargarismos y para lavar y descongestionar los ojos.
+hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. / La infusión se prepara con una cucharada de flores para 1 litro agua recién
+hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. / La infusión se prepara con una cucharada de flores para 1 litro agua recién
+hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. / La infusión se prepara con una cucharada de flores para 1 litro agua recién
+hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. / La infusión se prepara con una cucharada de flores para 1 litro agua recién
+hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. / La infusión se prepara con una cucharada de flores para 1 litro agua recién
+hervida; dejar reposar y filtrar: beber 1 taza 3 veces al día. Usar la misma infusión como gargarismos y para lavar y descongestionar los ojos.
 Usar como compresas calientes sobre pared abdominal en caso de cólicos. En
 hemorroides usar primero como vahos de asiento (cuando la infusión está
 caliente) y luego en baños de asiento (cuando la temperatura es tolerable sin
 quemarse).</t>
   </si>
   <si>
-    <t>antibacteriano / antiespasmódico / diurético suave, carminativo / anti-
+    <t>antibacteriano / antiespasmódico / diurético suave / carminativo / anti-
 inflamatorio / cicatrizante</t>
   </si>
   <si>
@@ -730,6 +1118,19 @@
 avalado por estudios clínicos.</t>
   </si>
   <si>
+    <t>Blancas y amarillas en el centro</t>
+  </si>
+  <si>
+    <t>15°C-23°C
+Resiste heladas</t>
+  </si>
+  <si>
+    <t>Franco arenosos, arcillosos, semi-húmedos-ligeros</t>
+  </si>
+  <si>
+    <t>Inicio apertura floral</t>
+  </si>
+  <si>
     <t>Hinojo</t>
   </si>
   <si>
@@ -756,7 +1157,10 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
-hervida: beber 1 taza 3 veces al día</t>
+hervida: beber 1 taza 3 veces al día / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día. / La infusión se prepara con 1 cucharada del vegetal para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>analgésico / antiespasmódico / carminativo / galactógeno</t>
@@ -778,6 +1182,12 @@
 evidencia científica.</t>
   </si>
   <si>
+    <t>Ricos en materia orgánica, ligeros y bien drenados</t>
+  </si>
+  <si>
+    <t>Verano-Otoño</t>
+  </si>
+  <si>
     <t>Llantén Menor</t>
   </si>
   <si>
@@ -808,9 +1218,29 @@
 Alternativamente puede dejarse macerando 1 manojo de hojas en 1 taza de agua
 fresca toda la noche y se bebe en la mañana siguiente; del zumo de hojas frescas
 machacadas o recién exprimidas puede usarse 5 – 10 gotas en una taza de agua
-fresca. / Se usa localmente la misma infusión de manera directa o mediante compresas;
+fresca. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.
+Alternativamente puede dejarse macerando 1 manojo de hojas en 1 taza de agua
+fresca toda la noche y se bebe en la mañana siguiente; del zumo de hojas frescas
+machacadas o recién exprimidas puede usarse 5 – 10 gotas en una taza de agua
+fresca. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.
+Alternativamente puede dejarse macerando 1 manojo de hojas en 1 taza de agua
+fresca toda la noche y se bebe en la mañana siguiente; del zumo de hojas frescas
+machacadas o recién exprimidas puede usarse 5 – 10 gotas en una taza de agua
+fresca. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.
+Alternativamente puede dejarse macerando 1 manojo de hojas en 1 taza de agua
+fresca toda la noche y se bebe en la mañana siguiente; del zumo de hojas frescas
+machacadas o recién exprimidas puede usarse 5 – 10 gotas en una taza de agua
+fresca. Se usa localmente la misma infusión de manera directa o mediante compresas;
 también puede aplicarse localmente compresas con el zumo de hojas frescas
-machacadas o recién exprimidas.</t>
+machacadas o recién exprimidas. / La infusión se prepara con 1 cucharada de hojas para 1 litro de agua recién
+hervida: beber 1 taza 3 veces al día.
+Alternativamente puede dejarse macerando 1 manojo de hojas en 1 taza de agua
+fresca toda la noche y se bebe en la mañana siguiente; del zumo de hojas frescas
+machacadas o recién exprimidas puede usarse 5 – 10 gotas en una taza de agua
+fresca.</t>
   </si>
   <si>
     <t>demulcente / emoliente / balsámico / cicatrizante / anti-inflamatorio</t>
@@ -829,6 +1259,22 @@
 científica.</t>
   </si>
   <si>
+    <t>Blanco o púrpura</t>
+  </si>
+  <si>
+    <t>20°C-35°C
+Resiste heladas, sequías moderadas</t>
+  </si>
+  <si>
+    <t>Semi-fértiles, no tan compactos, baja salinidad</t>
+  </si>
+  <si>
+    <t>2 vez por semana</t>
+  </si>
+  <si>
+    <t>Primavera</t>
+  </si>
+  <si>
     <t>Ortiga</t>
   </si>
   <si>
@@ -842,13 +1288,17 @@
   </si>
   <si>
     <t>La infusión se prepara con 2 cucharadas de hojas y ramas para 1 un litro de agua
-hirviendo: beber 1 taza 3 veces al día. / Se usa la misma infusión en lavados, emplastos o baños. Las ramas frescas se
+hirviendo: beber 1 taza 3 veces al día. / La infusión se prepara con 2 cucharadas de hojas y ramas para 1 un litro de agua
+hirviendo: beber 1 taza 3 veces al día. Se usa la misma infusión en lavados, emplastos o baños. Las ramas frescas se
 usan para ortigar (acción local de frotar o azotar con ortiga, la que debe comenzar
 por el lado derecho de la persona), por su efecto rubefaciente favorable en
 trastornos reumáticos, artríticos y la tonificación de músculos paralizados, seguido
 de frotación con agua helada y posterior arropamiento. / Se usa como decocción (cocimiento) con 40 gramos (2 cucharadas rasas) de raíz
 y rizomas para un litro de agua, se hierve 1 a 3 minutos: beber 1 taza 4 veces al
-día.</t>
+día. / La infusión se prepara con 2 cucharadas de hojas y ramas para 1 un litro de agua
+hirviendo: beber 1 taza 3 veces al día. / La infusión se prepara con 2 cucharadas de hojas y ramas para 1 un litro de agua
+hirviendo: beber 1 taza 3 veces al día. / La infusión se prepara con 2 cucharadas de hojas y ramas para 1 un litro de agua
+hirviendo: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>astringente / depurativo / diurético / rubefaciente / hemostático / anti-
@@ -870,6 +1320,22 @@
 anti-inflamatorio tiene alguna evidencia científica.</t>
   </si>
   <si>
+    <t>1.5 m</t>
+  </si>
+  <si>
+    <t>20°C-35°C
+Resiste heladas y sequías moderadas</t>
+  </si>
+  <si>
+    <t>Semisombra</t>
+  </si>
+  <si>
+    <t>Ricos en materia orgánica, nitrificados y bien drenados</t>
+  </si>
+  <si>
+    <t>Primavera-Verano</t>
+  </si>
+  <si>
     <t>Milenrama</t>
   </si>
   <si>
@@ -896,7 +1362,13 @@
   </si>
   <si>
     <t>La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
-recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. / Utilizar el doble de la cantidad de planta para el mismo volumen de agua.</t>
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. Utilizar el doble de la cantidad de planta para el mismo volumen de agua. / La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. Utilizar el doble de la cantidad de planta para el mismo volumen de agua. / La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. / La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. / La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. Utilizar el doble de la cantidad de planta para el mismo volumen de agua. / La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día. / La infusión se prepara con 2 cucharadas de la planta seca en 1 litro de agua
+recién hervida, dejar reposar 10 minutos: beber 1 taza 3 veces al día.</t>
   </si>
   <si>
     <t>antibacteriano / astringente / emenagogo / antiespasmódico / hemostático / febrifugo / anti-inflamatorio</t>
@@ -916,6 +1388,19 @@
 utensilios de aluminio.</t>
   </si>
   <si>
+    <t>Blanco, anaranjado, rosado a violeta</t>
+  </si>
+  <si>
+    <t>20°C-35°C
+Resiste heladas-sequías</t>
+  </si>
+  <si>
+    <t>Arenosos o arcillosos</t>
+  </si>
+  <si>
+    <t>Semillas y rizomas</t>
+  </si>
+  <si>
     <t>Zarzaparrilla</t>
   </si>
   <si>
@@ -927,7 +1412,10 @@
   </si>
   <si>
     <t>La infusión se prepara con 1 cucharada del vegetal para 1 taza de agua recién
-hervida: beber 1 taza 3 veces en el día. / Lavar la zona afectada con la misma infusión.</t>
+hervida: beber 1 taza 3 veces en el día. / La infusión se prepara con 1 cucharada del vegetal para 1 taza de agua recién
+hervida: beber 1 taza 3 veces en el día. / La infusión se prepara con 1 cucharada del vegetal para 1 taza de agua recién
+hervida: beber 1 taza 3 veces en el día. Lavar la zona afectada con la misma infusión. / La infusión se prepara con 1 cucharada del vegetal para 1 taza de agua recién
+hervida: beber 1 taza 3 veces en el día.</t>
   </si>
   <si>
     <t>depurativo / astringente / hemostático / antiséptico</t>
@@ -943,12 +1431,25 @@
 médico, infórmele que está usando esta hierba medicinal. Evite su preparación en
 utensilios de aluminio.</t>
   </si>
+  <si>
+    <t>Verde amarillentas y rojas por dentro</t>
+  </si>
+  <si>
+    <t>- - -
+Resiste heladas</t>
+  </si>
+  <si>
+    <t>Soleado-Semisombra</t>
+  </si>
+  <si>
+    <t>- - -</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -960,6 +1461,12 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -1012,7 +1519,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1022,20 +1529,29 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1256,13 +1772,14 @@
     <col customWidth="1" min="1" max="1" width="14.63"/>
     <col customWidth="1" min="2" max="2" width="16.13"/>
     <col customWidth="1" min="3" max="3" width="41.13"/>
-    <col customWidth="1" min="4" max="4" width="38.38"/>
-    <col customWidth="1" min="5" max="5" width="23.63"/>
-    <col customWidth="1" min="6" max="6" width="39.5"/>
-    <col customWidth="1" min="7" max="7" width="32.13"/>
-    <col customWidth="1" min="8" max="8" width="25.75"/>
-    <col customWidth="1" min="9" max="10" width="40.13"/>
-    <col customWidth="1" min="11" max="11" width="19.38"/>
+    <col customWidth="1" min="4" max="5" width="38.38"/>
+    <col customWidth="1" min="6" max="6" width="23.63"/>
+    <col customWidth="1" min="7" max="7" width="39.5"/>
+    <col customWidth="1" min="8" max="8" width="32.13"/>
+    <col customWidth="1" min="9" max="9" width="25.75"/>
+    <col customWidth="1" min="10" max="11" width="40.13"/>
+    <col customWidth="1" min="12" max="12" width="19.38"/>
+    <col customWidth="1" min="18" max="18" width="15.63"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1278,696 +1795,1485 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>29</v>
+      <c r="A3" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="S3" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="8" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="G4" s="5" t="s">
+      <c r="R4" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="S4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="I4" s="5" t="s">
+      <c r="T4" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="U4" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>40</v>
+      <c r="V4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="J5" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>51</v>
+      <c r="A5" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="M6" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>59</v>
+      <c r="N6" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="P6" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R6" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="S6" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="T6" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="U6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="W6" s="8" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>67</v>
+      <c r="A7" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="L7" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R7" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="T7" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="U7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W7" s="8" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="A8" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="L8" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N8" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="5" t="s">
+      <c r="O8" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="T8" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="U8" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="V8" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="W8" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>88</v>
-      </c>
+      <c r="A9" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="T9" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="U9" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W9" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="8"/>
+      <c r="AH9" s="8"/>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="A10" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T10" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="U10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V10" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W10" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="I11" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="A11" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="S11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T11" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="U11" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="V11" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W11" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>118</v>
-      </c>
+      <c r="A12" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>198</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="M12" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="O12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q12" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R12" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="S12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T12" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="U12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W12" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="M13" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O13" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="P13" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="Q13" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R13" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T13" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="U13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V13" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W13" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="G14" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H14" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I14" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="K14" s="5" t="s">
+      <c r="A14" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="M14" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>231</v>
+      </c>
+      <c r="O14" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="Q14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R14" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T14" s="8" t="s">
         <v>139</v>
       </c>
+      <c r="U14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V14" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="W14" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="3" t="s">
+      <c r="A15" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="L15" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="Q15" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R15" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T15" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="U15" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="V15" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="W15" s="8" t="s">
         <v>141</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>146</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="K16" s="5" t="s">
-        <v>161</v>
+      <c r="A16" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>252</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>253</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V16" s="10"/>
+      <c r="W16" s="8" t="s">
+        <v>264</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>169</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="K17" s="5" t="s">
-        <v>172</v>
+      <c r="A17" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="M17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="O17" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R17" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="S17" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="T17" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="U17" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W17" s="8" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>183</v>
+      <c r="A18" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="J18" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="K18" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="L18" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="M18" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="O18" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P18" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R18" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="S18" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="T18" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="U18" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="V18" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="W18" s="8" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="K19" s="5" t="s">
-        <v>191</v>
+      <c r="A19" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>298</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="S19" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="T19" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>194</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>198</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>199</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>200</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>51</v>
+      <c r="A20" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>311</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="L20" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M20" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="O20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P20" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="Q20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R20" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="S20" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="T20" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="U20" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="V20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W20" s="8" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="5" t="s">
-        <v>204</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>205</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>206</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>51</v>
+      <c r="A21" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>325</v>
+      </c>
+      <c r="J21" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="M21" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="P21" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="Q21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="R21" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="S21" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="U21" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="V21" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="W21" s="8" t="s">
+        <v>331</v>
       </c>
     </row>
   </sheetData>

</xml_diff>